<commit_message>
done with reading dates of excel sheet, also now it loads the questions of a determinate date
</commit_message>
<xml_diff>
--- a/trivia-front/back/Libro1.xlsx
+++ b/trivia-front/back/Libro1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diuca\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6B6686-6142-46EB-A29A-DCE1FD960F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C338894D-ABE5-452A-AE08-5BDD6EC35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BB0E2AA0-6AA7-4F59-A272-DF94D0BDC341}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>question</t>
   </si>
@@ -47,20 +48,145 @@
     <t>options</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b,c</t>
+    <t>date</t>
+  </si>
+  <si>
+    <t>What 90s boy band member bought Myspace in 2011?</t>
+  </si>
+  <si>
+    <t>Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Nick Lachey,Shawn Stockman,AJ McLean</t>
+  </si>
+  <si>
+    <t>What’s the name of Hagrid’s pet spider?</t>
+  </si>
+  <si>
+    <t>Aragog</t>
+  </si>
+  <si>
+    <t>Nigini,Crookshanks,Mosag</t>
+  </si>
+  <si>
+    <t>What’s the heaviest organ in the human body?</t>
+  </si>
+  <si>
+    <t>Brain,Skin,Heart</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>Which of these EU countries does not use the euro as its currency?</t>
+  </si>
+  <si>
+    <t>Poland,Denmark,Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All are correct</t>
+  </si>
+  <si>
+    <t>What element does the chemical symbol Au stand for?</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Salt,Magnesium,Silver</t>
+  </si>
+  <si>
+    <t>On average, how many seeds are located on the outside of a strawberry?</t>
+  </si>
+  <si>
+    <t>100,400,500</t>
+  </si>
+  <si>
+    <t>What is the oldest soft drink in the United States?</t>
+  </si>
+  <si>
+    <t>Dr. Pepper</t>
+  </si>
+  <si>
+    <t>Coca Cola,Pepsi,Canada Dry Ginger Ale</t>
+  </si>
+  <si>
+    <t>Central Perk</t>
+  </si>
+  <si>
+    <t>Java Park,Central Park Coffee,Central Park Roastery</t>
+  </si>
+  <si>
+    <t>Which country’s national animal is a unicorn?</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Denmark,New Zealand,France</t>
+  </si>
+  <si>
+    <t>What is the main ingredient in a falafel?</t>
+  </si>
+  <si>
+    <t>Lentil</t>
+  </si>
+  <si>
+    <t>Lentil,Broccoli,Split pea</t>
+  </si>
+  <si>
+    <r>
+      <t>What is the name of the coffee shop in the sitcom </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Friends</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>What color dresses do Chinese women traditionally wear on their wedding day?</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue,Gold,White</t>
+  </si>
+  <si>
+    <t>What is yellowtail fish called in Japanese?</t>
+  </si>
+  <si>
+    <t>Hamachi</t>
+  </si>
+  <si>
+    <t>Ahí,IkuraMaguro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-mm\-yyyy"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,16 +203,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,20 +259,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,90 +607,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C519661B-A16C-404E-8B23-8F15C88BDAF3}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="69" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="9">
+        <v>45166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="11">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4">
+        <v>200</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2404B6D6-C137-4173-BA25-82481C632484}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.28515625" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
started styling for front end
</commit_message>
<xml_diff>
--- a/trivia-front/back/Libro1.xlsx
+++ b/trivia-front/back/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diuca\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DECC222-E115-4FE9-9F9D-DC74ABE5123D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62B6572-0F2F-403D-B0BC-10710ECAA09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{BB0E2AA0-6AA7-4F59-A272-DF94D0BDC341}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BB0E2AA0-6AA7-4F59-A272-DF94D0BDC341}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>question</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Lentil</t>
-  </si>
-  <si>
-    <t>Lentil,Broccoli,Split pea</t>
   </si>
   <si>
     <r>
@@ -178,6 +175,9 @@
   <si>
     <t>Ahí,IkuraMaguro</t>
   </si>
+  <si>
+    <t>Broccoli,Split pea</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,14 +238,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF3A3A3A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -300,9 +292,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,7 +610,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,13 +637,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="9">
         <v>45166</v>
@@ -662,77 +651,157 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D3" s="11">
         <v>45165</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4">
+        <v>200</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45168</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
@@ -761,7 +830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2404B6D6-C137-4173-BA25-82481C632484}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -871,7 +942,7 @@
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>24</v>
@@ -905,7 +976,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5">
         <v>45164</v>
@@ -913,5 +984,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>